<commit_message>
Arquivo modificado sobre classificação e filtros
</commit_message>
<xml_diff>
--- a/filtros.xlsx
+++ b/filtros.xlsx
@@ -8,23 +8,45 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58383E9E-52D6-44AD-BFAB-EA81638E3E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AE14B8-DE93-4CF8-ABD4-98198CD4342A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="6" r:id="rId1"/>
-    <sheet name="Planilha3" sheetId="8" r:id="rId2"/>
+    <sheet name="Clientes" sheetId="6" r:id="rId1"/>
+    <sheet name="Hospitais" sheetId="8" r:id="rId2"/>
     <sheet name="Valores" sheetId="4" r:id="rId3"/>
-    <sheet name="Subtotais" sheetId="5" r:id="rId4"/>
-    <sheet name="Marca" sheetId="1" r:id="rId5"/>
+    <sheet name="Marca" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{92A975BF-4C12-4FCD-8E3D-D24CDB1A9197}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cadastro Nacional de Estabelecimentos de Saúde</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="516">
   <si>
     <t>Carros</t>
   </si>
@@ -1584,7 +1606,7 @@
     <numFmt numFmtId="165" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
     <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1608,14 +1630,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="7" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1631,12 +1660,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,24 +1701,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1725,9 +1748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1743,7 +1766,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3595007" y="29936"/>
-          <a:ext cx="5234668" cy="370114"/>
+          <a:ext cx="4967968" cy="236764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1778,8 +1801,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t>Exiba apenas os veículos com valores entre 40 e 70 mil</a:t>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>Usando filtros de dados, exiba apenas os veículos com valores entre 40 e 70 mil</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1794,22 +1817,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>80282</xdr:colOff>
+      <xdr:colOff>116794</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>39461</xdr:rowOff>
+      <xdr:rowOff>36285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>531813</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{024293F0-A6CD-46A6-9D0A-CD5EF3DC4D1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1817,8 +1840,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3585482" y="39461"/>
-          <a:ext cx="7968343" cy="408214"/>
+          <a:off x="3617232" y="36285"/>
+          <a:ext cx="4693331" cy="217715"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1853,84 +1876,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t>Aplique os subtotais ordenados por marca do veículo e com o subtotal do preço.</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1800"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>116794</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>36286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>531813</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3617232" y="36286"/>
-          <a:ext cx="4693331" cy="376464"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t>Faça uma classificação por marca de veículos</a:t>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>Faça uma classificação de dados em ordem crescente por marca de veículos </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2230,236 +2177,236 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>35486</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>5134445569</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>456789</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>5134859632</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>800</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>365897</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>5198547896</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>44569</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>5198856932</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>630</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>25697</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>5134658774</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>490</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>123456</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>5134859535</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>11235</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>5186352478</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>670</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>24589</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>5135356585</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>920</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>21236</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>5135466998</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>1800</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>32548</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>5134556628</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>2500</v>
       </c>
     </row>
@@ -2469,11 +2416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA3EC39-8A8F-411C-8BA1-7C412052EF44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA3EC39-8A8F-411C-8BA1-7C412052EF44}">
   <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2469,7 @@
       <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2542,7 +2489,7 @@
       <c r="E3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2562,7 +2509,7 @@
       <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2582,7 +2529,7 @@
       <c r="E5" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2602,7 +2549,7 @@
       <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2622,7 +2569,7 @@
       <c r="E7" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2642,7 +2589,7 @@
       <c r="E8" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2662,7 +2609,7 @@
       <c r="E9" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2682,7 +2629,7 @@
       <c r="E10" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2702,7 +2649,7 @@
       <c r="E11" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2722,7 +2669,7 @@
       <c r="E12" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2742,7 +2689,7 @@
       <c r="E13" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2762,7 +2709,7 @@
       <c r="E14" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2782,7 +2729,7 @@
       <c r="E15" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2802,7 +2749,7 @@
       <c r="E16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2822,7 +2769,7 @@
       <c r="E17" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2842,7 +2789,7 @@
       <c r="E18" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2862,7 +2809,7 @@
       <c r="E19" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2882,7 +2829,7 @@
       <c r="E20" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2902,7 +2849,7 @@
       <c r="E21" t="s">
         <v>110</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2922,7 +2869,7 @@
       <c r="E22" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2942,7 +2889,7 @@
       <c r="E23" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2962,7 +2909,7 @@
       <c r="E24" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -2982,7 +2929,7 @@
       <c r="E25" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3002,7 +2949,7 @@
       <c r="E26" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3022,7 +2969,7 @@
       <c r="E27" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3042,7 +2989,7 @@
       <c r="E28" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3062,7 +3009,7 @@
       <c r="E29" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3082,7 +3029,7 @@
       <c r="E30" t="s">
         <v>126</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3102,7 +3049,7 @@
       <c r="E31" t="s">
         <v>128</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3122,7 +3069,7 @@
       <c r="E32" t="s">
         <v>130</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3142,7 +3089,7 @@
       <c r="E33" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3162,7 +3109,7 @@
       <c r="E34" t="s">
         <v>135</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3182,7 +3129,7 @@
       <c r="E35" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3202,7 +3149,7 @@
       <c r="E36" t="s">
         <v>139</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3222,7 +3169,7 @@
       <c r="E37" t="s">
         <v>81</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3242,7 +3189,7 @@
       <c r="E38" t="s">
         <v>142</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3262,7 +3209,7 @@
       <c r="E39" t="s">
         <v>144</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3282,7 +3229,7 @@
       <c r="E40" t="s">
         <v>146</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3302,7 +3249,7 @@
       <c r="E41" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3322,7 +3269,7 @@
       <c r="E42" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3342,7 +3289,7 @@
       <c r="E43" t="s">
         <v>151</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3362,7 +3309,7 @@
       <c r="E44" t="s">
         <v>153</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3382,7 +3329,7 @@
       <c r="E45" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3402,7 +3349,7 @@
       <c r="E46" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3422,7 +3369,7 @@
       <c r="E47" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3442,7 +3389,7 @@
       <c r="E48" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3462,7 +3409,7 @@
       <c r="E49" t="s">
         <v>81</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3482,7 +3429,7 @@
       <c r="E50" t="s">
         <v>64</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3502,7 +3449,7 @@
       <c r="E51" t="s">
         <v>162</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3522,7 +3469,7 @@
       <c r="E52" t="s">
         <v>165</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3542,7 +3489,7 @@
       <c r="E53" t="s">
         <v>167</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3562,7 +3509,7 @@
       <c r="E54" t="s">
         <v>72</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3582,7 +3529,7 @@
       <c r="E55" t="s">
         <v>113</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3602,7 +3549,7 @@
       <c r="E56" t="s">
         <v>171</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3622,7 +3569,7 @@
       <c r="E57" t="s">
         <v>173</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F57" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3642,7 +3589,7 @@
       <c r="E58" t="s">
         <v>175</v>
       </c>
-      <c r="F58" s="11">
+      <c r="F58" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3662,7 +3609,7 @@
       <c r="E59" t="s">
         <v>177</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F59" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3682,7 +3629,7 @@
       <c r="E60" t="s">
         <v>179</v>
       </c>
-      <c r="F60" s="11">
+      <c r="F60" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3702,7 +3649,7 @@
       <c r="E61" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="11">
+      <c r="F61" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3722,7 +3669,7 @@
       <c r="E62" t="s">
         <v>183</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3742,7 +3689,7 @@
       <c r="E63" t="s">
         <v>186</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3762,7 +3709,7 @@
       <c r="E64" t="s">
         <v>69</v>
       </c>
-      <c r="F64" s="11">
+      <c r="F64" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3782,7 +3729,7 @@
       <c r="E65" t="s">
         <v>189</v>
       </c>
-      <c r="F65" s="11">
+      <c r="F65" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3802,7 +3749,7 @@
       <c r="E66" t="s">
         <v>69</v>
       </c>
-      <c r="F66" s="11">
+      <c r="F66" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3822,7 +3769,7 @@
       <c r="E67" t="s">
         <v>171</v>
       </c>
-      <c r="F67" s="11">
+      <c r="F67" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3842,7 +3789,7 @@
       <c r="E68" t="s">
         <v>194</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3862,7 +3809,7 @@
       <c r="E69" t="s">
         <v>135</v>
       </c>
-      <c r="F69" s="11">
+      <c r="F69" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3882,7 +3829,7 @@
       <c r="E70" t="s">
         <v>132</v>
       </c>
-      <c r="F70" s="11">
+      <c r="F70" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3902,7 +3849,7 @@
       <c r="E71" t="s">
         <v>198</v>
       </c>
-      <c r="F71" s="11">
+      <c r="F71" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3922,7 +3869,7 @@
       <c r="E72" t="s">
         <v>171</v>
       </c>
-      <c r="F72" s="11">
+      <c r="F72" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3942,7 +3889,7 @@
       <c r="E73" t="s">
         <v>202</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3962,7 +3909,7 @@
       <c r="E74" t="s">
         <v>96</v>
       </c>
-      <c r="F74" s="11">
+      <c r="F74" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -3982,7 +3929,7 @@
       <c r="E75" t="s">
         <v>96</v>
       </c>
-      <c r="F75" s="11">
+      <c r="F75" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4002,7 +3949,7 @@
       <c r="E76" t="s">
         <v>206</v>
       </c>
-      <c r="F76" s="11">
+      <c r="F76" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4022,7 +3969,7 @@
       <c r="E77" t="s">
         <v>194</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4042,7 +3989,7 @@
       <c r="E78" t="s">
         <v>135</v>
       </c>
-      <c r="F78" s="11">
+      <c r="F78" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4062,7 +4009,7 @@
       <c r="E79" t="s">
         <v>171</v>
       </c>
-      <c r="F79" s="11">
+      <c r="F79" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4082,7 +4029,7 @@
       <c r="E80" t="s">
         <v>132</v>
       </c>
-      <c r="F80" s="11">
+      <c r="F80" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4102,7 +4049,7 @@
       <c r="E81" t="s">
         <v>132</v>
       </c>
-      <c r="F81" s="11">
+      <c r="F81" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4122,7 +4069,7 @@
       <c r="E82" t="s">
         <v>202</v>
       </c>
-      <c r="F82" s="11">
+      <c r="F82" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4142,7 +4089,7 @@
       <c r="E83" t="s">
         <v>214</v>
       </c>
-      <c r="F83" s="11">
+      <c r="F83" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4162,7 +4109,7 @@
       <c r="E84" t="s">
         <v>81</v>
       </c>
-      <c r="F84" s="11">
+      <c r="F84" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4182,7 +4129,7 @@
       <c r="E85" t="s">
         <v>217</v>
       </c>
-      <c r="F85" s="11">
+      <c r="F85" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4202,7 +4149,7 @@
       <c r="E86" t="s">
         <v>219</v>
       </c>
-      <c r="F86" s="11">
+      <c r="F86" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4222,7 +4169,7 @@
       <c r="E87" t="s">
         <v>221</v>
       </c>
-      <c r="F87" s="11">
+      <c r="F87" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4242,7 +4189,7 @@
       <c r="E88" t="s">
         <v>223</v>
       </c>
-      <c r="F88" s="11">
+      <c r="F88" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4262,7 +4209,7 @@
       <c r="E89" t="s">
         <v>225</v>
       </c>
-      <c r="F89" s="11">
+      <c r="F89" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4282,7 +4229,7 @@
       <c r="E90" t="s">
         <v>227</v>
       </c>
-      <c r="F90" s="11">
+      <c r="F90" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4302,7 +4249,7 @@
       <c r="E91" t="s">
         <v>230</v>
       </c>
-      <c r="F91" s="11">
+      <c r="F91" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4322,7 +4269,7 @@
       <c r="E92" t="s">
         <v>121</v>
       </c>
-      <c r="F92" s="11">
+      <c r="F92" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4342,7 +4289,7 @@
       <c r="E93" t="s">
         <v>233</v>
       </c>
-      <c r="F93" s="11">
+      <c r="F93" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4362,7 +4309,7 @@
       <c r="E94" t="s">
         <v>235</v>
       </c>
-      <c r="F94" s="11">
+      <c r="F94" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4382,7 +4329,7 @@
       <c r="E95" t="s">
         <v>237</v>
       </c>
-      <c r="F95" s="11">
+      <c r="F95" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4402,7 +4349,7 @@
       <c r="E96" t="s">
         <v>142</v>
       </c>
-      <c r="F96" s="11">
+      <c r="F96" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4422,7 +4369,7 @@
       <c r="E97" t="s">
         <v>240</v>
       </c>
-      <c r="F97" s="11">
+      <c r="F97" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4442,7 +4389,7 @@
       <c r="E98" t="s">
         <v>242</v>
       </c>
-      <c r="F98" s="11">
+      <c r="F98" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4462,7 +4409,7 @@
       <c r="E99" t="s">
         <v>244</v>
       </c>
-      <c r="F99" s="11">
+      <c r="F99" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4482,7 +4429,7 @@
       <c r="E100" t="s">
         <v>130</v>
       </c>
-      <c r="F100" s="11">
+      <c r="F100" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4502,7 +4449,7 @@
       <c r="E101" t="s">
         <v>247</v>
       </c>
-      <c r="F101" s="11">
+      <c r="F101" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4522,7 +4469,7 @@
       <c r="E102" t="s">
         <v>249</v>
       </c>
-      <c r="F102" s="11">
+      <c r="F102" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4542,7 +4489,7 @@
       <c r="E103" t="s">
         <v>72</v>
       </c>
-      <c r="F103" s="11">
+      <c r="F103" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4562,7 +4509,7 @@
       <c r="E104" t="s">
         <v>252</v>
       </c>
-      <c r="F104" s="11">
+      <c r="F104" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4582,7 +4529,7 @@
       <c r="E105" t="s">
         <v>254</v>
       </c>
-      <c r="F105" s="11">
+      <c r="F105" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4602,7 +4549,7 @@
       <c r="E106" t="s">
         <v>257</v>
       </c>
-      <c r="F106" s="11">
+      <c r="F106" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4622,7 +4569,7 @@
       <c r="E107" t="s">
         <v>259</v>
       </c>
-      <c r="F107" s="11">
+      <c r="F107" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4642,7 +4589,7 @@
       <c r="E108" t="s">
         <v>173</v>
       </c>
-      <c r="F108" s="11">
+      <c r="F108" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4662,7 +4609,7 @@
       <c r="E109" t="s">
         <v>235</v>
       </c>
-      <c r="F109" s="11">
+      <c r="F109" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4682,7 +4629,7 @@
       <c r="E110" t="s">
         <v>221</v>
       </c>
-      <c r="F110" s="11">
+      <c r="F110" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4702,7 +4649,7 @@
       <c r="E111" t="s">
         <v>179</v>
       </c>
-      <c r="F111" s="11">
+      <c r="F111" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4722,7 +4669,7 @@
       <c r="E112" t="s">
         <v>265</v>
       </c>
-      <c r="F112" s="11">
+      <c r="F112" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4742,7 +4689,7 @@
       <c r="E113" t="s">
         <v>267</v>
       </c>
-      <c r="F113" s="11">
+      <c r="F113" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4762,7 +4709,7 @@
       <c r="E114" t="s">
         <v>151</v>
       </c>
-      <c r="F114" s="11">
+      <c r="F114" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4782,7 +4729,7 @@
       <c r="E115" t="s">
         <v>270</v>
       </c>
-      <c r="F115" s="11">
+      <c r="F115" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4802,7 +4749,7 @@
       <c r="E116" t="s">
         <v>272</v>
       </c>
-      <c r="F116" s="11">
+      <c r="F116" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4822,7 +4769,7 @@
       <c r="E117" t="s">
         <v>115</v>
       </c>
-      <c r="F117" s="11">
+      <c r="F117" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4842,7 +4789,7 @@
       <c r="E118" t="s">
         <v>275</v>
       </c>
-      <c r="F118" s="11">
+      <c r="F118" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4862,7 +4809,7 @@
       <c r="E119" t="s">
         <v>277</v>
       </c>
-      <c r="F119" s="11">
+      <c r="F119" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4882,7 +4829,7 @@
       <c r="E120" t="s">
         <v>194</v>
       </c>
-      <c r="F120" s="11">
+      <c r="F120" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4902,7 +4849,7 @@
       <c r="E121" t="s">
         <v>135</v>
       </c>
-      <c r="F121" s="11">
+      <c r="F121" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4922,7 +4869,7 @@
       <c r="E122" t="s">
         <v>130</v>
       </c>
-      <c r="F122" s="11">
+      <c r="F122" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4942,7 +4889,7 @@
       <c r="E123" t="s">
         <v>281</v>
       </c>
-      <c r="F123" s="11">
+      <c r="F123" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4962,7 +4909,7 @@
       <c r="E124" t="s">
         <v>283</v>
       </c>
-      <c r="F124" s="11">
+      <c r="F124" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -4982,7 +4929,7 @@
       <c r="E125" t="s">
         <v>285</v>
       </c>
-      <c r="F125" s="11">
+      <c r="F125" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5002,7 +4949,7 @@
       <c r="E126" t="s">
         <v>287</v>
       </c>
-      <c r="F126" s="11">
+      <c r="F126" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5022,7 +4969,7 @@
       <c r="E127" t="s">
         <v>289</v>
       </c>
-      <c r="F127" s="11">
+      <c r="F127" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5042,7 +4989,7 @@
       <c r="E128" t="s">
         <v>291</v>
       </c>
-      <c r="F128" s="11">
+      <c r="F128" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5062,7 +5009,7 @@
       <c r="E129" t="s">
         <v>293</v>
       </c>
-      <c r="F129" s="11">
+      <c r="F129" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5082,7 +5029,7 @@
       <c r="E130" t="s">
         <v>244</v>
       </c>
-      <c r="F130" s="11">
+      <c r="F130" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5102,7 +5049,7 @@
       <c r="E131" t="s">
         <v>171</v>
       </c>
-      <c r="F131" s="11">
+      <c r="F131" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5122,7 +5069,7 @@
       <c r="E132" t="s">
         <v>151</v>
       </c>
-      <c r="F132" s="11">
+      <c r="F132" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5142,7 +5089,7 @@
       <c r="E133" t="s">
         <v>298</v>
       </c>
-      <c r="F133" s="11">
+      <c r="F133" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5162,7 +5109,7 @@
       <c r="E134" t="s">
         <v>300</v>
       </c>
-      <c r="F134" s="11">
+      <c r="F134" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5182,7 +5129,7 @@
       <c r="E135" t="s">
         <v>302</v>
       </c>
-      <c r="F135" s="11">
+      <c r="F135" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5202,7 +5149,7 @@
       <c r="E136" t="s">
         <v>304</v>
       </c>
-      <c r="F136" s="11">
+      <c r="F136" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5222,7 +5169,7 @@
       <c r="E137" t="s">
         <v>162</v>
       </c>
-      <c r="F137" s="11">
+      <c r="F137" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5242,7 +5189,7 @@
       <c r="E138" t="s">
         <v>307</v>
       </c>
-      <c r="F138" s="11">
+      <c r="F138" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5262,7 +5209,7 @@
       <c r="E139" t="s">
         <v>81</v>
       </c>
-      <c r="F139" s="11">
+      <c r="F139" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5282,7 +5229,7 @@
       <c r="E140" t="s">
         <v>310</v>
       </c>
-      <c r="F140" s="11">
+      <c r="F140" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5302,7 +5249,7 @@
       <c r="E141" t="s">
         <v>312</v>
       </c>
-      <c r="F141" s="11">
+      <c r="F141" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5322,7 +5269,7 @@
       <c r="E142" t="s">
         <v>64</v>
       </c>
-      <c r="F142" s="11">
+      <c r="F142" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5342,7 +5289,7 @@
       <c r="E143" t="s">
         <v>198</v>
       </c>
-      <c r="F143" s="11">
+      <c r="F143" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5362,7 +5309,7 @@
       <c r="E144" t="s">
         <v>104</v>
       </c>
-      <c r="F144" s="11">
+      <c r="F144" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5382,7 +5329,7 @@
       <c r="E145" t="s">
         <v>317</v>
       </c>
-      <c r="F145" s="11">
+      <c r="F145" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5402,7 +5349,7 @@
       <c r="E146" t="s">
         <v>135</v>
       </c>
-      <c r="F146" s="11">
+      <c r="F146" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5422,7 +5369,7 @@
       <c r="E147" t="s">
         <v>320</v>
       </c>
-      <c r="F147" s="11">
+      <c r="F147" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5442,7 +5389,7 @@
       <c r="E148" t="s">
         <v>320</v>
       </c>
-      <c r="F148" s="11">
+      <c r="F148" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5462,7 +5409,7 @@
       <c r="E149" t="s">
         <v>104</v>
       </c>
-      <c r="F149" s="11">
+      <c r="F149" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5482,7 +5429,7 @@
       <c r="E150" t="s">
         <v>130</v>
       </c>
-      <c r="F150" s="11">
+      <c r="F150" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5502,7 +5449,7 @@
       <c r="E151" t="s">
         <v>325</v>
       </c>
-      <c r="F151" s="11">
+      <c r="F151" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5522,7 +5469,7 @@
       <c r="E152" t="s">
         <v>327</v>
       </c>
-      <c r="F152" s="11">
+      <c r="F152" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5542,7 +5489,7 @@
       <c r="E153" t="s">
         <v>310</v>
       </c>
-      <c r="F153" s="11">
+      <c r="F153" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5562,7 +5509,7 @@
       <c r="E154" t="s">
         <v>281</v>
       </c>
-      <c r="F154" s="11">
+      <c r="F154" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5582,7 +5529,7 @@
       <c r="E155" t="s">
         <v>104</v>
       </c>
-      <c r="F155" s="11">
+      <c r="F155" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5602,7 +5549,7 @@
       <c r="E156" t="s">
         <v>244</v>
       </c>
-      <c r="F156" s="11">
+      <c r="F156" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5622,7 +5569,7 @@
       <c r="E157" t="s">
         <v>69</v>
       </c>
-      <c r="F157" s="11">
+      <c r="F157" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5642,7 +5589,7 @@
       <c r="E158" t="s">
         <v>96</v>
       </c>
-      <c r="F158" s="11">
+      <c r="F158" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5662,7 +5609,7 @@
       <c r="E159" t="s">
         <v>335</v>
       </c>
-      <c r="F159" s="11">
+      <c r="F159" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5682,7 +5629,7 @@
       <c r="E160" t="s">
         <v>337</v>
       </c>
-      <c r="F160" s="11">
+      <c r="F160" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5702,7 +5649,7 @@
       <c r="E161" t="s">
         <v>101</v>
       </c>
-      <c r="F161" s="11">
+      <c r="F161" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5722,7 +5669,7 @@
       <c r="E162" t="s">
         <v>304</v>
       </c>
-      <c r="F162" s="11">
+      <c r="F162" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5742,7 +5689,7 @@
       <c r="E163" t="s">
         <v>130</v>
       </c>
-      <c r="F163" s="11">
+      <c r="F163" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5762,7 +5709,7 @@
       <c r="E164" t="s">
         <v>342</v>
       </c>
-      <c r="F164" s="11">
+      <c r="F164" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5782,7 +5729,7 @@
       <c r="E165" t="s">
         <v>135</v>
       </c>
-      <c r="F165" s="11">
+      <c r="F165" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5802,7 +5749,7 @@
       <c r="E166" t="s">
         <v>64</v>
       </c>
-      <c r="F166" s="11">
+      <c r="F166" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5822,7 +5769,7 @@
       <c r="E167" t="s">
         <v>144</v>
       </c>
-      <c r="F167" s="11">
+      <c r="F167" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5842,7 +5789,7 @@
       <c r="E168" t="s">
         <v>347</v>
       </c>
-      <c r="F168" s="11">
+      <c r="F168" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5862,7 +5809,7 @@
       <c r="E169" t="s">
         <v>349</v>
       </c>
-      <c r="F169" s="11">
+      <c r="F169" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5882,7 +5829,7 @@
       <c r="E170" t="s">
         <v>104</v>
       </c>
-      <c r="F170" s="11">
+      <c r="F170" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5902,7 +5849,7 @@
       <c r="E171" t="s">
         <v>352</v>
       </c>
-      <c r="F171" s="11">
+      <c r="F171" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5922,7 +5869,7 @@
       <c r="E172" t="s">
         <v>354</v>
       </c>
-      <c r="F172" s="11">
+      <c r="F172" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5942,7 +5889,7 @@
       <c r="E173" t="s">
         <v>356</v>
       </c>
-      <c r="F173" s="11">
+      <c r="F173" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5962,7 +5909,7 @@
       <c r="E174" t="s">
         <v>358</v>
       </c>
-      <c r="F174" s="11">
+      <c r="F174" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -5982,7 +5929,7 @@
       <c r="E175" t="s">
         <v>221</v>
       </c>
-      <c r="F175" s="11">
+      <c r="F175" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6002,7 +5949,7 @@
       <c r="E176" t="s">
         <v>135</v>
       </c>
-      <c r="F176" s="11">
+      <c r="F176" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6022,7 +5969,7 @@
       <c r="E177" t="s">
         <v>361</v>
       </c>
-      <c r="F177" s="11">
+      <c r="F177" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6042,7 +5989,7 @@
       <c r="E178" t="s">
         <v>93</v>
       </c>
-      <c r="F178" s="11">
+      <c r="F178" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6062,7 +6009,7 @@
       <c r="E179" t="s">
         <v>364</v>
       </c>
-      <c r="F179" s="11">
+      <c r="F179" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6082,7 +6029,7 @@
       <c r="E180" t="s">
         <v>132</v>
       </c>
-      <c r="F180" s="11">
+      <c r="F180" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6102,7 +6049,7 @@
       <c r="E181" t="s">
         <v>367</v>
       </c>
-      <c r="F181" s="11">
+      <c r="F181" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6122,7 +6069,7 @@
       <c r="E182" t="s">
         <v>369</v>
       </c>
-      <c r="F182" s="11">
+      <c r="F182" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6142,7 +6089,7 @@
       <c r="E183" t="s">
         <v>247</v>
       </c>
-      <c r="F183" s="11">
+      <c r="F183" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6162,7 +6109,7 @@
       <c r="E184" t="s">
         <v>371</v>
       </c>
-      <c r="F184" s="11">
+      <c r="F184" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6182,7 +6129,7 @@
       <c r="E185" t="s">
         <v>373</v>
       </c>
-      <c r="F185" s="11">
+      <c r="F185" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6202,7 +6149,7 @@
       <c r="E186" t="s">
         <v>375</v>
       </c>
-      <c r="F186" s="11">
+      <c r="F186" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6222,7 +6169,7 @@
       <c r="E187" t="s">
         <v>377</v>
       </c>
-      <c r="F187" s="11">
+      <c r="F187" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6242,7 +6189,7 @@
       <c r="E188" t="s">
         <v>162</v>
       </c>
-      <c r="F188" s="11">
+      <c r="F188" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6262,7 +6209,7 @@
       <c r="E189" t="s">
         <v>380</v>
       </c>
-      <c r="F189" s="11">
+      <c r="F189" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6282,7 +6229,7 @@
       <c r="E190" t="s">
         <v>382</v>
       </c>
-      <c r="F190" s="11">
+      <c r="F190" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6302,7 +6249,7 @@
       <c r="E191" t="s">
         <v>96</v>
       </c>
-      <c r="F191" s="11">
+      <c r="F191" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6322,7 +6269,7 @@
       <c r="E192" t="s">
         <v>72</v>
       </c>
-      <c r="F192" s="11">
+      <c r="F192" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6342,7 +6289,7 @@
       <c r="E193" t="s">
         <v>144</v>
       </c>
-      <c r="F193" s="11">
+      <c r="F193" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6362,7 +6309,7 @@
       <c r="E194" t="s">
         <v>81</v>
       </c>
-      <c r="F194" s="11">
+      <c r="F194" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6382,7 +6329,7 @@
       <c r="E195" t="s">
         <v>96</v>
       </c>
-      <c r="F195" s="11">
+      <c r="F195" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6402,7 +6349,7 @@
       <c r="E196" t="s">
         <v>389</v>
       </c>
-      <c r="F196" s="11">
+      <c r="F196" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6422,7 +6369,7 @@
       <c r="E197" t="s">
         <v>64</v>
       </c>
-      <c r="F197" s="11">
+      <c r="F197" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6442,7 +6389,7 @@
       <c r="E198" t="s">
         <v>392</v>
       </c>
-      <c r="F198" s="11">
+      <c r="F198" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6462,7 +6409,7 @@
       <c r="E199" t="s">
         <v>194</v>
       </c>
-      <c r="F199" s="11">
+      <c r="F199" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6482,7 +6429,7 @@
       <c r="E200" t="s">
         <v>76</v>
       </c>
-      <c r="F200" s="11">
+      <c r="F200" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6502,7 +6449,7 @@
       <c r="E201" t="s">
         <v>395</v>
       </c>
-      <c r="F201" s="11">
+      <c r="F201" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6522,7 +6469,7 @@
       <c r="E202" t="s">
         <v>96</v>
       </c>
-      <c r="F202" s="11">
+      <c r="F202" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6542,7 +6489,7 @@
       <c r="E203" t="s">
         <v>130</v>
       </c>
-      <c r="F203" s="11">
+      <c r="F203" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6562,7 +6509,7 @@
       <c r="E204" t="s">
         <v>399</v>
       </c>
-      <c r="F204" s="11">
+      <c r="F204" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6582,7 +6529,7 @@
       <c r="E205" t="s">
         <v>69</v>
       </c>
-      <c r="F205" s="11">
+      <c r="F205" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6602,7 +6549,7 @@
       <c r="E206" t="s">
         <v>81</v>
       </c>
-      <c r="F206" s="11">
+      <c r="F206" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6622,7 +6569,7 @@
       <c r="E207" t="s">
         <v>194</v>
       </c>
-      <c r="F207" s="11">
+      <c r="F207" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6642,7 +6589,7 @@
       <c r="E208" t="s">
         <v>76</v>
       </c>
-      <c r="F208" s="11">
+      <c r="F208" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6662,7 +6609,7 @@
       <c r="E209" t="s">
         <v>130</v>
       </c>
-      <c r="F209" s="11">
+      <c r="F209" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6682,7 +6629,7 @@
       <c r="E210" t="s">
         <v>153</v>
       </c>
-      <c r="F210" s="11">
+      <c r="F210" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6702,7 +6649,7 @@
       <c r="E211" t="s">
         <v>81</v>
       </c>
-      <c r="F211" s="11">
+      <c r="F211" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6722,7 +6669,7 @@
       <c r="E212" t="s">
         <v>281</v>
       </c>
-      <c r="F212" s="11">
+      <c r="F212" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6742,7 +6689,7 @@
       <c r="E213" t="s">
         <v>389</v>
       </c>
-      <c r="F213" s="11">
+      <c r="F213" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6762,7 +6709,7 @@
       <c r="E214" t="s">
         <v>171</v>
       </c>
-      <c r="F214" s="11">
+      <c r="F214" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6782,7 +6729,7 @@
       <c r="E215" t="s">
         <v>337</v>
       </c>
-      <c r="F215" s="11">
+      <c r="F215" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6802,7 +6749,7 @@
       <c r="E216" t="s">
         <v>412</v>
       </c>
-      <c r="F216" s="11">
+      <c r="F216" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6822,7 +6769,7 @@
       <c r="E217" t="s">
         <v>130</v>
       </c>
-      <c r="F217" s="11">
+      <c r="F217" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6842,7 +6789,7 @@
       <c r="E218" t="s">
         <v>389</v>
       </c>
-      <c r="F218" s="11">
+      <c r="F218" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6862,7 +6809,7 @@
       <c r="E219" t="s">
         <v>416</v>
       </c>
-      <c r="F219" s="11">
+      <c r="F219" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6882,7 +6829,7 @@
       <c r="E220" t="s">
         <v>162</v>
       </c>
-      <c r="F220" s="11">
+      <c r="F220" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6902,7 +6849,7 @@
       <c r="E221" t="s">
         <v>135</v>
       </c>
-      <c r="F221" s="11">
+      <c r="F221" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6922,7 +6869,7 @@
       <c r="E222" t="s">
         <v>135</v>
       </c>
-      <c r="F222" s="11">
+      <c r="F222" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6942,7 +6889,7 @@
       <c r="E223" t="s">
         <v>421</v>
       </c>
-      <c r="F223" s="11">
+      <c r="F223" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6962,7 +6909,7 @@
       <c r="E224" t="s">
         <v>113</v>
       </c>
-      <c r="F224" s="11">
+      <c r="F224" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -6982,7 +6929,7 @@
       <c r="E225" t="s">
         <v>300</v>
       </c>
-      <c r="F225" s="11">
+      <c r="F225" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7002,7 +6949,7 @@
       <c r="E226" t="s">
         <v>96</v>
       </c>
-      <c r="F226" s="11">
+      <c r="F226" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7022,7 +6969,7 @@
       <c r="E227" t="s">
         <v>426</v>
       </c>
-      <c r="F227" s="11">
+      <c r="F227" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7042,7 +6989,7 @@
       <c r="E228" t="s">
         <v>72</v>
       </c>
-      <c r="F228" s="11">
+      <c r="F228" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7062,7 +7009,7 @@
       <c r="E229" t="s">
         <v>130</v>
       </c>
-      <c r="F229" s="11">
+      <c r="F229" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7082,7 +7029,7 @@
       <c r="E230" t="s">
         <v>81</v>
       </c>
-      <c r="F230" s="11">
+      <c r="F230" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7102,7 +7049,7 @@
       <c r="E231" t="s">
         <v>431</v>
       </c>
-      <c r="F231" s="11">
+      <c r="F231" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7122,7 +7069,7 @@
       <c r="E232" t="s">
         <v>310</v>
       </c>
-      <c r="F232" s="11">
+      <c r="F232" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7142,7 +7089,7 @@
       <c r="E233" t="s">
         <v>392</v>
       </c>
-      <c r="F233" s="11">
+      <c r="F233" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7162,7 +7109,7 @@
       <c r="E234" t="s">
         <v>434</v>
       </c>
-      <c r="F234" s="11">
+      <c r="F234" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7182,7 +7129,7 @@
       <c r="E235" t="s">
         <v>64</v>
       </c>
-      <c r="F235" s="11">
+      <c r="F235" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7202,7 +7149,7 @@
       <c r="E236" t="s">
         <v>104</v>
       </c>
-      <c r="F236" s="11">
+      <c r="F236" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7222,7 +7169,7 @@
       <c r="E237" t="s">
         <v>132</v>
       </c>
-      <c r="F237" s="11">
+      <c r="F237" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7242,7 +7189,7 @@
       <c r="E238" t="s">
         <v>186</v>
       </c>
-      <c r="F238" s="11">
+      <c r="F238" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7262,7 +7209,7 @@
       <c r="E239" t="s">
         <v>440</v>
       </c>
-      <c r="F239" s="11">
+      <c r="F239" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7282,7 +7229,7 @@
       <c r="E240" t="s">
         <v>151</v>
       </c>
-      <c r="F240" s="11">
+      <c r="F240" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7302,7 +7249,7 @@
       <c r="E241" t="s">
         <v>151</v>
       </c>
-      <c r="F241" s="11">
+      <c r="F241" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7322,7 +7269,7 @@
       <c r="E242" t="s">
         <v>244</v>
       </c>
-      <c r="F242" s="11">
+      <c r="F242" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7342,7 +7289,7 @@
       <c r="E243" t="s">
         <v>426</v>
       </c>
-      <c r="F243" s="11">
+      <c r="F243" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7362,7 +7309,7 @@
       <c r="E244" t="s">
         <v>67</v>
       </c>
-      <c r="F244" s="11">
+      <c r="F244" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7382,7 +7329,7 @@
       <c r="E245" t="s">
         <v>135</v>
       </c>
-      <c r="F245" s="11">
+      <c r="F245" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7402,7 +7349,7 @@
       <c r="E246" t="s">
         <v>64</v>
       </c>
-      <c r="F246" s="11">
+      <c r="F246" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7422,7 +7369,7 @@
       <c r="E247" t="s">
         <v>64</v>
       </c>
-      <c r="F247" s="11">
+      <c r="F247" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7442,7 +7389,7 @@
       <c r="E248" t="s">
         <v>450</v>
       </c>
-      <c r="F248" s="11">
+      <c r="F248" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7462,7 +7409,7 @@
       <c r="E249" t="s">
         <v>153</v>
       </c>
-      <c r="F249" s="11">
+      <c r="F249" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7482,7 +7429,7 @@
       <c r="E250" t="s">
         <v>162</v>
       </c>
-      <c r="F250" s="11">
+      <c r="F250" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7502,7 +7449,7 @@
       <c r="E251" t="s">
         <v>454</v>
       </c>
-      <c r="F251" s="11">
+      <c r="F251" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7522,7 +7469,7 @@
       <c r="E252" t="s">
         <v>244</v>
       </c>
-      <c r="F252" s="11">
+      <c r="F252" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7542,7 +7489,7 @@
       <c r="E253" t="s">
         <v>81</v>
       </c>
-      <c r="F253" s="11">
+      <c r="F253" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7562,7 +7509,7 @@
       <c r="E254" t="s">
         <v>233</v>
       </c>
-      <c r="F254" s="11">
+      <c r="F254" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7582,7 +7529,7 @@
       <c r="E255" t="s">
         <v>72</v>
       </c>
-      <c r="F255" s="11">
+      <c r="F255" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7602,7 +7549,7 @@
       <c r="E256" t="s">
         <v>460</v>
       </c>
-      <c r="F256" s="11">
+      <c r="F256" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7622,7 +7569,7 @@
       <c r="E257" t="s">
         <v>462</v>
       </c>
-      <c r="F257" s="11">
+      <c r="F257" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7642,7 +7589,7 @@
       <c r="E258" t="s">
         <v>464</v>
       </c>
-      <c r="F258" s="11">
+      <c r="F258" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7662,7 +7609,7 @@
       <c r="E259" t="s">
         <v>64</v>
       </c>
-      <c r="F259" s="11">
+      <c r="F259" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7682,7 +7629,7 @@
       <c r="E260" t="s">
         <v>104</v>
       </c>
-      <c r="F260" s="11">
+      <c r="F260" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7702,7 +7649,7 @@
       <c r="E261" t="s">
         <v>186</v>
       </c>
-      <c r="F261" s="11">
+      <c r="F261" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7722,7 +7669,7 @@
       <c r="E262" t="s">
         <v>142</v>
       </c>
-      <c r="F262" s="11">
+      <c r="F262" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7742,7 +7689,7 @@
       <c r="E263" t="s">
         <v>81</v>
       </c>
-      <c r="F263" s="11">
+      <c r="F263" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7762,7 +7709,7 @@
       <c r="E264" t="s">
         <v>389</v>
       </c>
-      <c r="F264" s="11">
+      <c r="F264" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7782,7 +7729,7 @@
       <c r="E265" t="s">
         <v>389</v>
       </c>
-      <c r="F265" s="11">
+      <c r="F265" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7802,7 +7749,7 @@
       <c r="E266" t="s">
         <v>473</v>
       </c>
-      <c r="F266" s="11">
+      <c r="F266" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7822,7 +7769,7 @@
       <c r="E267" t="s">
         <v>475</v>
       </c>
-      <c r="F267" s="11">
+      <c r="F267" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7842,7 +7789,7 @@
       <c r="E268" t="s">
         <v>477</v>
       </c>
-      <c r="F268" s="11">
+      <c r="F268" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7862,7 +7809,7 @@
       <c r="E269" t="s">
         <v>479</v>
       </c>
-      <c r="F269" s="11">
+      <c r="F269" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7882,7 +7829,7 @@
       <c r="E270" t="s">
         <v>481</v>
       </c>
-      <c r="F270" s="11">
+      <c r="F270" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7902,7 +7849,7 @@
       <c r="E271" t="s">
         <v>483</v>
       </c>
-      <c r="F271" s="11">
+      <c r="F271" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7922,7 +7869,7 @@
       <c r="E272" t="s">
         <v>485</v>
       </c>
-      <c r="F272" s="11">
+      <c r="F272" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7942,7 +7889,7 @@
       <c r="E273" t="s">
         <v>487</v>
       </c>
-      <c r="F273" s="11">
+      <c r="F273" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7962,7 +7909,7 @@
       <c r="E274" t="s">
         <v>489</v>
       </c>
-      <c r="F274" s="11">
+      <c r="F274" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -7982,7 +7929,7 @@
       <c r="E275" t="s">
         <v>132</v>
       </c>
-      <c r="F275" s="11">
+      <c r="F275" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8002,7 +7949,7 @@
       <c r="E276" t="s">
         <v>135</v>
       </c>
-      <c r="F276" s="11">
+      <c r="F276" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8022,7 +7969,7 @@
       <c r="E277" t="s">
         <v>493</v>
       </c>
-      <c r="F277" s="11">
+      <c r="F277" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8042,7 +7989,7 @@
       <c r="E278" t="s">
         <v>64</v>
       </c>
-      <c r="F278" s="11">
+      <c r="F278" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8062,7 +8009,7 @@
       <c r="E279" t="s">
         <v>496</v>
       </c>
-      <c r="F279" s="11">
+      <c r="F279" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8082,7 +8029,7 @@
       <c r="E280" t="s">
         <v>135</v>
       </c>
-      <c r="F280" s="11">
+      <c r="F280" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8102,7 +8049,7 @@
       <c r="E281" t="s">
         <v>64</v>
       </c>
-      <c r="F281" s="11">
+      <c r="F281" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8122,7 +8069,7 @@
       <c r="E282" t="s">
         <v>500</v>
       </c>
-      <c r="F282" s="11">
+      <c r="F282" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8142,7 +8089,7 @@
       <c r="E283" t="s">
         <v>310</v>
       </c>
-      <c r="F283" s="11">
+      <c r="F283" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8162,7 +8109,7 @@
       <c r="E284" t="s">
         <v>503</v>
       </c>
-      <c r="F284" s="11">
+      <c r="F284" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8182,7 +8129,7 @@
       <c r="E285" t="s">
         <v>206</v>
       </c>
-      <c r="F285" s="11">
+      <c r="F285" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8202,7 +8149,7 @@
       <c r="E286" t="s">
         <v>81</v>
       </c>
-      <c r="F286" s="11">
+      <c r="F286" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8222,7 +8169,7 @@
       <c r="E287" t="s">
         <v>281</v>
       </c>
-      <c r="F287" s="11">
+      <c r="F287" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8242,7 +8189,7 @@
       <c r="E288" t="s">
         <v>500</v>
       </c>
-      <c r="F288" s="11">
+      <c r="F288" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8262,7 +8209,7 @@
       <c r="E289" t="s">
         <v>509</v>
       </c>
-      <c r="F289" s="11">
+      <c r="F289" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8282,7 +8229,7 @@
       <c r="E290" t="s">
         <v>130</v>
       </c>
-      <c r="F290" s="11">
+      <c r="F290" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8302,7 +8249,7 @@
       <c r="E291" t="s">
         <v>104</v>
       </c>
-      <c r="F291" s="11">
+      <c r="F291" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8322,7 +8269,7 @@
       <c r="E292" t="s">
         <v>96</v>
       </c>
-      <c r="F292" s="11">
+      <c r="F292" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8342,7 +8289,7 @@
       <c r="E293" t="s">
         <v>96</v>
       </c>
-      <c r="F293" s="11">
+      <c r="F293" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8362,7 +8309,7 @@
       <c r="E294" t="s">
         <v>202</v>
       </c>
-      <c r="F294" s="11">
+      <c r="F294" s="4">
         <v>43342</v>
       </c>
     </row>
@@ -8382,12 +8329,13 @@
       <c r="E295" t="s">
         <v>123</v>
       </c>
-      <c r="F295" s="11">
+      <c r="F295" s="4">
         <v>43342</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8395,8 +8343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338A7FB8-571D-47EF-BE24-7CC869A59E77}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8408,12 +8356,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8700,11 +8648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3322242-7ADE-4BD2-85C5-6E3F6FCDC0BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8716,320 +8664,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1017</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1008</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1001</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1014</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1015</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1012</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3">
-        <v>38000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1011</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3">
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1016</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1013</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3">
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1002</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="3">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1009</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1010</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="3">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1003</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="3">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1004</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3">
-        <v>89000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1005</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3">
-        <v>112000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1006</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3">
-        <v>162000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>1007</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3">
-        <v>200000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="decimal" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VC errou" error="não coloque numeros negativos" sqref="D3:D20" xr:uid="{B6653EB3-E069-4537-8DF5-8C9D4F613C98}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="codigo errado" error="colocar numeros entre 1000 e 2000" sqref="A3:A20" xr:uid="{FC2BB210-E4EC-483C-A54A-9E51C64A8E1D}">
-      <formula1>1000</formula1>
-      <formula2>2000</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>